<commit_message>
Schablone + Variable-default eingebaut
</commit_message>
<xml_diff>
--- a/Schablonen/ZweiEbenenThorax.xlsx
+++ b/Schablonen/ZweiEbenenThorax.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71C505B-7C2A-4F5C-9607-5A6273CD98BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D5CE65-BB6E-4DDF-BB32-377F67029D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E9688302-5921-49C1-BE4B-315E9EEA5948}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="370">
   <si>
     <t>Gliederung</t>
   </si>
@@ -1145,9 +1145,6 @@
   </si>
   <si>
     <t>%O2% freie Luft unter der Zwerchfellkuppe</t>
-  </si>
-  <si>
-    <t>Beurteilung</t>
   </si>
 </sst>
 </file>
@@ -1540,11 +1537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD863459-8DC2-4F08-8B8A-0734853F8245}">
-  <dimension ref="A1:P127"/>
+  <dimension ref="A1:P126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A128" sqref="A128"/>
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,7 +1675,7 @@
       </c>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -2525,7 +2521,7 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
@@ -2581,7 +2577,7 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2607,7 +2603,7 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2663,7 +2659,7 @@
       </c>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
@@ -2693,7 +2689,7 @@
       </c>
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
@@ -2805,7 +2801,7 @@
       </c>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
@@ -2839,7 +2835,7 @@
       </c>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
@@ -2873,7 +2869,7 @@
       </c>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
@@ -2905,7 +2901,7 @@
       </c>
       <c r="P47" s="2"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3369,7 +3365,7 @@
       </c>
       <c r="P62" s="2"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
@@ -3401,7 +3397,7 @@
       </c>
       <c r="P63" s="2"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -4638,11 +4634,6 @@
       </c>
       <c r="O126" t="s">
         <v>368</v>
-      </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added function to check each excel row for parsing errors
</commit_message>
<xml_diff>
--- a/Schablonen/ZweiEbenenThorax.xlsx
+++ b/Schablonen/ZweiEbenenThorax.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amar\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D5CE65-BB6E-4DDF-BB32-377F67029D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340DE8FD-078A-484E-9C3A-94CC5ABDCDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E9688302-5921-49C1-BE4B-315E9EEA5948}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="41180" windowHeight="21100" xr2:uid="{E9688302-5921-49C1-BE4B-315E9EEA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="388">
   <si>
     <t>Gliederung</t>
   </si>
@@ -109,9 +109,6 @@
     <t>von ...</t>
   </si>
   <si>
-    <t>ZVK [von %I1% ]%I2%[: %I3%]</t>
-  </si>
-  <si>
     <t>I2</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>I4</t>
   </si>
   <si>
-    <t>ZVK [von %I4% ]%I5%[: %I6%]</t>
-  </si>
-  <si>
     <t>I5</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
     <t>I7</t>
   </si>
   <si>
-    <t>Shaldon-Katheter [von %I7%] %I8%[: %I9%.]</t>
-  </si>
-  <si>
     <t>I8</t>
   </si>
   <si>
@@ -175,9 +166,6 @@
     <t>I10</t>
   </si>
   <si>
-    <t>Shaldon-Katheter [von %I10%] %I11%[: %I12%.]</t>
-  </si>
-  <si>
     <t>I11</t>
   </si>
   <si>
@@ -190,9 +178,6 @@
     <t>I13</t>
   </si>
   <si>
-    <t>Schleuse [von %I13%] jugulär[: %I14%.]</t>
-  </si>
-  <si>
     <t>I14</t>
   </si>
   <si>
@@ -205,9 +190,6 @@
     <t>I15</t>
   </si>
   <si>
-    <t>Pleuradrainage [von %I15%][: %I16%.]</t>
-  </si>
-  <si>
     <t>I16</t>
   </si>
   <si>
@@ -220,9 +202,6 @@
     <t>I17</t>
   </si>
   <si>
-    <t>Pleuradrainage [von %I17%][: %I18%.]</t>
-  </si>
-  <si>
     <t>I18</t>
   </si>
   <si>
@@ -235,9 +214,6 @@
     <t>I19</t>
   </si>
   <si>
-    <t>Pleuradrainage [von %I19%][: %I20%.]</t>
-  </si>
-  <si>
     <t>I20</t>
   </si>
   <si>
@@ -250,18 +226,12 @@
     <t>I21</t>
   </si>
   <si>
-    <t>Mediastinaldrainage %I21%</t>
-  </si>
-  <si>
     <t>Perikarddrainage</t>
   </si>
   <si>
     <t>I22</t>
   </si>
   <si>
-    <t>Perikarddrainage %I22%</t>
-  </si>
-  <si>
     <t>Magensonde</t>
   </si>
   <si>
@@ -271,9 +241,6 @@
     <t>I23</t>
   </si>
   <si>
-    <t>Magensonde[: %I23%.]</t>
-  </si>
-  <si>
     <t>ETT</t>
   </si>
   <si>
@@ -283,9 +250,6 @@
     <t>I24</t>
   </si>
   <si>
-    <t>ETT[: %I24%,] [%I25% cm suprakarinal endend.]</t>
-  </si>
-  <si>
     <t>I25</t>
   </si>
   <si>
@@ -301,9 +265,6 @@
     <t>I26</t>
   </si>
   <si>
-    <t>Port-System [von %I26% ][%I27%][: %I28% der Katheterspitze.]</t>
-  </si>
-  <si>
     <t>I27</t>
   </si>
   <si>
@@ -334,9 +295,6 @@
     <t>SM / ICD / Event-Recorder;Event-Rekorder;Eventrekorder;Eventrecorder</t>
   </si>
   <si>
-    <t>[%I29%-]Aggregat [%I30% pektoral,] [%I31% konnektierte(s) Sondenkabel,] [%I32% im Summationsbild. ]</t>
-  </si>
-  <si>
     <t>I30</t>
   </si>
   <si>
@@ -379,9 +337,6 @@
     <t>mit ...</t>
   </si>
   <si>
-    <t>Postoperativer Status [nach %I33%. ]</t>
-  </si>
-  <si>
     <t>Klappen-OP</t>
   </si>
   <si>
@@ -397,9 +352,6 @@
     <t>TAVI, LAVI;AKE;AKR;MKE;MKR</t>
   </si>
   <si>
-    <t xml:space="preserve">%I34% erfolgt. </t>
-  </si>
-  <si>
     <t>Sternalcerclagen</t>
   </si>
   <si>
@@ -409,9 +361,6 @@
     <t>insgesamt ... Cerclagen</t>
   </si>
   <si>
-    <t>[%I35% ]Sternalcerclagen[, %I36%.]</t>
-  </si>
-  <si>
     <t>I36</t>
   </si>
   <si>
@@ -589,36 +538,6 @@
     <t>auf Höhe der … dorsalen Rippe</t>
   </si>
   <si>
-    <t>regelrechte Lage %Z1%</t>
-  </si>
-  <si>
-    <t>homogen gewölbt %Z2%</t>
-  </si>
-  <si>
-    <t>scharf abgrenzbar %Z3%</t>
-  </si>
-  <si>
-    <t>geringe Inspirationstiefe %Z4% auf Höhe der %Z5%. dorsalen Rippe</t>
-  </si>
-  <si>
-    <t>Zwerchfellhochstand %Z6%</t>
-  </si>
-  <si>
-    <t>Zwerchfelltiefstand %Z7%</t>
-  </si>
-  <si>
-    <t>abgeflacht %Z8%</t>
-  </si>
-  <si>
-    <t>unscharf abgrenzbar %Z9%</t>
-  </si>
-  <si>
-    <t>nicht abgrenzbar %Z10%</t>
-  </si>
-  <si>
-    <t>Zwerchfellbuckel %Z11%</t>
-  </si>
-  <si>
     <t>ZW1</t>
   </si>
   <si>
@@ -634,21 +553,6 @@
     <t>ZW5</t>
   </si>
   <si>
-    <t>spitz konfiguriert %ZW1%</t>
-  </si>
-  <si>
-    <t>frei einsehbar %ZW2%</t>
-  </si>
-  <si>
-    <t>aufgespreizt %ZW3%</t>
-  </si>
-  <si>
-    <t>ausgerundet %ZW4%</t>
-  </si>
-  <si>
-    <t>verlegt %ZW5%</t>
-  </si>
-  <si>
     <t>\n\nZwechfellrandwinkel: \n</t>
   </si>
   <si>
@@ -715,39 +619,12 @@
     <t>\n\nPleura:\n</t>
   </si>
   <si>
-    <t>der Lunge allseits anliegend %P1%</t>
-  </si>
-  <si>
-    <t>Pleuraerguss %P4%</t>
-  </si>
-  <si>
-    <t>fokale Raumforderung %P6%</t>
-  </si>
-  <si>
-    <t>verkalkte Plaques %P7%</t>
-  </si>
-  <si>
-    <t>keine fokale Verdickung %P8%</t>
-  </si>
-  <si>
-    <t>der Lunge abgehoben %P2% (maximale Dehiszenz ca. %P3% cm)</t>
-  </si>
-  <si>
-    <t>verdickt %P5%</t>
-  </si>
-  <si>
     <t>Mediastinum</t>
   </si>
   <si>
     <t>\n\nMediastinum:\n</t>
   </si>
   <si>
-    <t>mittelständig</t>
-  </si>
-  <si>
-    <t>normal breit</t>
-  </si>
-  <si>
     <t>Trachea mittelständig und normal breit</t>
   </si>
   <si>
@@ -802,18 +679,12 @@
     <t>geringe Inspirationstiefe des Zwerchfells; geringe Inspirationstiefe</t>
   </si>
   <si>
-    <t>regeltechter Carinawinkel</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
     <t>nach …</t>
   </si>
   <si>
-    <t>nach %M1% verlagert</t>
-  </si>
-  <si>
     <t>M2</t>
   </si>
   <si>
@@ -823,9 +694,6 @@
     <t>M3</t>
   </si>
   <si>
-    <t>%M2% Mediastinum nach %M3% verbreitert</t>
-  </si>
-  <si>
     <t>\n\nHerz:\n</t>
   </si>
   <si>
@@ -835,9 +703,6 @@
     <t>… cm</t>
   </si>
   <si>
-    <t>verbreiterter Retrosternalraum (%M4% cm)</t>
-  </si>
-  <si>
     <t>Hili</t>
   </si>
   <si>
@@ -892,15 +757,6 @@
     <t>links … mm</t>
   </si>
   <si>
-    <t>erweitere Pulmonalarterie[ rechts %H2% mm][ links %H3% mm]</t>
-  </si>
-  <si>
-    <t>[ links %H3% mm][ links %H3% mm]</t>
-  </si>
-  <si>
-    <t>nodulär konfiguriert %H1%</t>
-  </si>
-  <si>
     <t>\n\nLunge:\n</t>
   </si>
   <si>
@@ -958,9 +814,6 @@
     <t>… positivem Bronchopneumogramm</t>
   </si>
   <si>
-    <t>Konsolidierung [im %L1% ] %L2% [%L3% positivem Bronchopneumogramm]</t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
@@ -994,12 +847,6 @@
     <t>L11</t>
   </si>
   <si>
-    <t>Milchglastrübungen [im %L4%]</t>
-  </si>
-  <si>
-    <t>Dystelektasen [im %L5%]</t>
-  </si>
-  <si>
     <t>OL;ML;UL</t>
   </si>
   <si>
@@ -1012,27 +859,9 @@
     <t>retikuläre/noduläre/retikonoduläre</t>
   </si>
   <si>
-    <t>interstitelle %L7% Zeichnungsvermehrung [im %L6%]</t>
-  </si>
-  <si>
-    <t>Rundherd [im %L8%]</t>
-  </si>
-  <si>
-    <t>Raumforderung [im %L9%]</t>
-  </si>
-  <si>
-    <t>Kaverne [im %L10%]</t>
-  </si>
-  <si>
-    <t>bullöse Lungengerüstveränderungen [im %L11%]</t>
-  </si>
-  <si>
     <t>\n\nSkelett:\n</t>
   </si>
   <si>
-    <t>Unauffällige Darstellung der miterfassten Skelettabschnitte</t>
-  </si>
-  <si>
     <t>Skelett unauffällig</t>
   </si>
   <si>
@@ -1057,15 +886,6 @@
     <t>…  Ende</t>
   </si>
   <si>
-    <t>%S3%</t>
-  </si>
-  <si>
-    <t>Osteoponie %S1%</t>
-  </si>
-  <si>
-    <t>Frakturen %S2%</t>
-  </si>
-  <si>
     <t>\n\nWeichteile:\n</t>
   </si>
   <si>
@@ -1084,12 +904,6 @@
     <t>Weitere Auffälligkeiten der Weichteile</t>
   </si>
   <si>
-    <t>Unauffällige Darstellung der miterfassten Weichteile</t>
-  </si>
-  <si>
-    <t>asymmetrischer Mammaschatten %W1%</t>
-  </si>
-  <si>
     <t>W1</t>
   </si>
   <si>
@@ -1099,9 +913,6 @@
     <t>W2</t>
   </si>
   <si>
-    <t>%W2%</t>
-  </si>
-  <si>
     <t>Oberbauch</t>
   </si>
   <si>
@@ -1129,9 +940,6 @@
     <t>unter der … Zwerchfellkuppe</t>
   </si>
   <si>
-    <t>distendierte Darmschlingen %o1%</t>
-  </si>
-  <si>
     <t>O2</t>
   </si>
   <si>
@@ -1141,10 +949,256 @@
     <t>O3</t>
   </si>
   <si>
-    <t>%O3% in Projektion auf das Gallenblasenbett</t>
-  </si>
-  <si>
-    <t>%O2% freie Luft unter der Zwerchfellkuppe</t>
+    <t>ZVK [von %I1% ]%I2%[: %I3%]\n</t>
+  </si>
+  <si>
+    <t>ZVK [von %I4% ]%I5%[: %I6%]\n</t>
+  </si>
+  <si>
+    <t>Shaldon-Katheter [von %I7%] %I8%[: %I9%.]\n</t>
+  </si>
+  <si>
+    <t>Shaldon-Katheter [von %I10%] %I11%[: %I12%.]\n</t>
+  </si>
+  <si>
+    <t>Schleuse [von %I13%] jugulär[: %I14%.]\n</t>
+  </si>
+  <si>
+    <t>Pleuradrainage [von %I15%][: %I16%.]\n</t>
+  </si>
+  <si>
+    <t>Pleuradrainage [von %I17%][: %I18%.]\n</t>
+  </si>
+  <si>
+    <t>Pleuradrainage [von %I19%][: %I20%.]\n</t>
+  </si>
+  <si>
+    <t>Mediastinaldrainage %I21%\n</t>
+  </si>
+  <si>
+    <t>Perikarddrainage %I22%\n</t>
+  </si>
+  <si>
+    <t>Magensonde[: %I23%.]\n</t>
+  </si>
+  <si>
+    <t>ETT[: %I24%,] [%I25% cm suprakarinal endend.]\n</t>
+  </si>
+  <si>
+    <t>Port-System [von %I26% ][%I27%][: %I28% der Katheterspitze.]\n</t>
+  </si>
+  <si>
+    <t>[%I29%-]Aggregat [%I30% pektoral,] [%I31% konnektierte(s) Sondenkabel,] [%I32% im Summationsbild. ]\n</t>
+  </si>
+  <si>
+    <t>Postoperativer Status [nach %I33%. ]\n</t>
+  </si>
+  <si>
+    <t>%I34% erfolgt. \n</t>
+  </si>
+  <si>
+    <t>[%I35% ]Sternalcerclagen[, %I36%.]\n</t>
+  </si>
+  <si>
+    <t>regelrechte Lage %Z1%\n</t>
+  </si>
+  <si>
+    <t>homogen gewölbt %Z2%\n</t>
+  </si>
+  <si>
+    <t>scharf abgrenzbar %Z3%\n</t>
+  </si>
+  <si>
+    <t>geringe Inspirationstiefe %Z4% auf Höhe der %Z5%. dorsalen Rippe\n</t>
+  </si>
+  <si>
+    <t>Zwerchfellhochstand %Z6%\n</t>
+  </si>
+  <si>
+    <t>Zwerchfelltiefstand %Z7%\n</t>
+  </si>
+  <si>
+    <t>abgeflacht %Z8%\n</t>
+  </si>
+  <si>
+    <t>unscharf abgrenzbar %Z9%\n</t>
+  </si>
+  <si>
+    <t>nicht abgrenzbar %Z10%\n</t>
+  </si>
+  <si>
+    <t>Zwerchfellbuckel %Z11%\n</t>
+  </si>
+  <si>
+    <t>spitz konfiguriert %ZW1%\n</t>
+  </si>
+  <si>
+    <t>frei einsehbar %ZW2%\n</t>
+  </si>
+  <si>
+    <t>aufgespreizt %ZW3%\n</t>
+  </si>
+  <si>
+    <t>ausgerundet %ZW4%\n</t>
+  </si>
+  <si>
+    <t>verlegt %ZW5%\n</t>
+  </si>
+  <si>
+    <t>der Lunge allseits anliegend %P1%\n</t>
+  </si>
+  <si>
+    <t>der Lunge abgehoben %P2% (maximale Dehiszenz ca. %P3% cm)\n</t>
+  </si>
+  <si>
+    <t>Pleuraerguss %P4%\n</t>
+  </si>
+  <si>
+    <t>verdickt %P5%\n</t>
+  </si>
+  <si>
+    <t>fokale Raumforderung %P6%\n</t>
+  </si>
+  <si>
+    <t>verkalkte Plaques %P7%\n</t>
+  </si>
+  <si>
+    <t>keine fokale Verdickung %P8%\n</t>
+  </si>
+  <si>
+    <t>mittelständig\n</t>
+  </si>
+  <si>
+    <t>normal breit\n</t>
+  </si>
+  <si>
+    <t>Trachea mittelständig und normal breit\n</t>
+  </si>
+  <si>
+    <t>regeltechter Carinawinkel\n</t>
+  </si>
+  <si>
+    <t>frei einsehbares aortopulmonales Fenster\n</t>
+  </si>
+  <si>
+    <t>regelrechte Weite des Retrosternalraumes\n</t>
+  </si>
+  <si>
+    <t>nach %M1% verlagert\n</t>
+  </si>
+  <si>
+    <t>%M2% Mediastinum nach %M3% verbreitert\n</t>
+  </si>
+  <si>
+    <t>Carina aufgespreizt\n</t>
+  </si>
+  <si>
+    <t>konkav konfiguriertes aortopulmonales Fenster\n</t>
+  </si>
+  <si>
+    <t>verbreiterter Retrosternalraum (%M4% cm)\n</t>
+  </si>
+  <si>
+    <t>normal groß\n</t>
+  </si>
+  <si>
+    <t>regelrechte Konfiguration\n</t>
+  </si>
+  <si>
+    <t>vergrößert\n</t>
+  </si>
+  <si>
+    <t>aortal konfiguriert\n</t>
+  </si>
+  <si>
+    <t>zeltförmiger Herzsilhouette\n</t>
+  </si>
+  <si>
+    <t>vaskulär konfiguriert\n</t>
+  </si>
+  <si>
+    <t>nodulär konfiguriert %H1%\n</t>
+  </si>
+  <si>
+    <t>erweitere Pulmonalarterie[ rechts %H2% mm][ links %H3% mm]\n</t>
+  </si>
+  <si>
+    <t>[ links %H3% mm][ links %H3% mm]\n</t>
+  </si>
+  <si>
+    <t>verwaschene Hilusstrukturen\n</t>
+  </si>
+  <si>
+    <t>Konsolidierung [im %L1% ] %L2% [%L3% positivem Bronchopneumogramm]\n</t>
+  </si>
+  <si>
+    <t>Milchglastrübungen [im %L4%]\n</t>
+  </si>
+  <si>
+    <t>Dystelektasen [im %L5%]\n</t>
+  </si>
+  <si>
+    <t>interstitelle %L7% Zeichnungsvermehrung [im %L6%]\n</t>
+  </si>
+  <si>
+    <t>Rundherd [im %L8%]\n</t>
+  </si>
+  <si>
+    <t>Raumforderung [im %L9%]\n</t>
+  </si>
+  <si>
+    <t>Kaverne [im %L10%]\n</t>
+  </si>
+  <si>
+    <t>bullöse Lungengerüstveränderungen [im %L11%]\n</t>
+  </si>
+  <si>
+    <t>unscharfe pulmonalvenöse Gefäßzeichnung\n</t>
+  </si>
+  <si>
+    <t>basoapikale Umverteilung\n</t>
+  </si>
+  <si>
+    <t>bronchiales Cuffing\n</t>
+  </si>
+  <si>
+    <t>Kerley-B Linien\n</t>
+  </si>
+  <si>
+    <t>Unauffällige Darstellung der miterfassten Skelettabschnitte\n</t>
+  </si>
+  <si>
+    <t>Osteoponie %S1%\n</t>
+  </si>
+  <si>
+    <t>Frakturen %S2%\n</t>
+  </si>
+  <si>
+    <t>%S3%\n</t>
+  </si>
+  <si>
+    <t>Unauffällige Darstellung der miterfassten Weichteile\n</t>
+  </si>
+  <si>
+    <t>asymmetrischer Mammaschatten %W1%\n</t>
+  </si>
+  <si>
+    <t>%W2%\n</t>
+  </si>
+  <si>
+    <t>unauffällig\n</t>
+  </si>
+  <si>
+    <t>distendierte Darmschlingen %o1%\n</t>
+  </si>
+  <si>
+    <t>%O2% freie Luft unter der Zwerchfellkuppe\n</t>
+  </si>
+  <si>
+    <t>%O3% in Projektion auf das Gallenblasenbett\n</t>
+  </si>
+  <si>
+    <t>Beurteilung</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1279,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1241,7 +1295,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1537,33 +1591,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD863459-8DC2-4F08-8B8A-0734853F8245}">
-  <dimension ref="A1:P126"/>
+  <dimension ref="A1:P127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" customWidth="1"/>
-    <col min="11" max="11" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" customWidth="1"/>
-    <col min="15" max="15" width="40.7109375" customWidth="1"/>
-    <col min="16" max="16" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="45.81640625" customWidth="1"/>
+    <col min="4" max="4" width="42.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.54296875" customWidth="1"/>
+    <col min="11" max="11" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.453125" customWidth="1"/>
+    <col min="13" max="13" width="13.54296875" customWidth="1"/>
+    <col min="14" max="14" width="17.7265625" customWidth="1"/>
+    <col min="15" max="15" width="40.7265625" customWidth="1"/>
+    <col min="16" max="16" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1580,7 +1634,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -1601,7 +1655,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>11</v>
@@ -1613,23 +1667,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1639,28 +1693,28 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>15</v>
@@ -1668,21 +1722,21 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
@@ -1701,7 +1755,7 @@
       </c>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1719,22 +1773,22 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>14</v>
@@ -1749,11 +1803,11 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -1781,11 +1835,11 @@
         <v>23</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>24</v>
+        <v>304</v>
       </c>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1796,20 +1850,20 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1820,27 +1874,27 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1848,7 +1902,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>21</v>
@@ -1861,11 +1915,11 @@
         <v>23</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>34</v>
+        <v>305</v>
       </c>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1876,20 +1930,20 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1900,27 +1954,27 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1928,7 +1982,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>21</v>
@@ -1941,11 +1995,11 @@
         <v>23</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>40</v>
+        <v>306</v>
       </c>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1956,20 +2010,20 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1980,27 +2034,27 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -2008,7 +2062,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>21</v>
@@ -2021,11 +2075,11 @@
         <v>23</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>46</v>
+        <v>307</v>
       </c>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2036,20 +2090,20 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2060,27 +2114,27 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2088,7 +2142,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>21</v>
@@ -2101,11 +2155,11 @@
         <v>23</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>51</v>
+        <v>308</v>
       </c>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2116,27 +2170,27 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2144,7 +2198,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>21</v>
@@ -2157,11 +2211,11 @@
         <v>23</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>56</v>
+        <v>309</v>
       </c>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2172,27 +2226,27 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2200,7 +2254,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>21</v>
@@ -2213,11 +2267,11 @@
         <v>23</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2228,27 +2282,27 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2256,7 +2310,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>21</v>
@@ -2269,11 +2323,11 @@
         <v>23</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>66</v>
+        <v>311</v>
       </c>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2284,27 +2338,27 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2312,29 +2366,29 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2" t="s">
-        <v>71</v>
+        <v>312</v>
       </c>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -2342,29 +2396,29 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2" t="s">
-        <v>74</v>
+        <v>313</v>
       </c>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2372,29 +2426,29 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="K29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2" t="s">
-        <v>78</v>
+        <v>314</v>
       </c>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -2402,22 +2456,22 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="K30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="M30" s="3"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2" t="s">
-        <v>82</v>
+        <v>315</v>
       </c>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2428,27 +2482,27 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -2456,7 +2510,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>21</v>
@@ -2469,11 +2523,11 @@
         <v>23</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>88</v>
+        <v>316</v>
       </c>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2484,20 +2538,20 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2508,27 +2562,27 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -2536,22 +2590,22 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2" t="s">
-        <v>99</v>
+        <v>317</v>
       </c>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2562,7 +2616,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>21</v>
@@ -2577,7 +2631,7 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2588,22 +2642,22 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2614,27 +2668,27 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -2642,31 +2696,31 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>114</v>
+        <v>318</v>
       </c>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -2674,29 +2728,29 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2" t="s">
-        <v>120</v>
+        <v>319</v>
       </c>
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -2704,22 +2758,22 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>124</v>
+        <v>320</v>
       </c>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2730,20 +2784,20 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>16</v>
       </c>
@@ -2761,20 +2815,20 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="P43" s="2"/>
     </row>
-    <row r="44" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>14</v>
@@ -2784,31 +2838,31 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2" t="s">
-        <v>184</v>
+        <v>321</v>
       </c>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>14</v>
@@ -2818,31 +2872,31 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2" t="s">
-        <v>185</v>
+        <v>322</v>
       </c>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>14</v>
@@ -2852,31 +2906,31 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2" t="s">
-        <v>186</v>
+        <v>323</v>
       </c>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>254</v>
+        <v>213</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -2884,24 +2938,24 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="6" t="s">
-        <v>187</v>
+        <v>324</v>
       </c>
       <c r="P47" s="2"/>
     </row>
-    <row r="48" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2912,27 +2966,27 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="O48" s="6"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -2940,31 +2994,31 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="7" t="s">
-        <v>188</v>
+        <v>325</v>
       </c>
       <c r="P49" s="2"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -2972,31 +3026,31 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="7" t="s">
-        <v>189</v>
+        <v>326</v>
       </c>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -3004,31 +3058,31 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="7" t="s">
-        <v>190</v>
+        <v>327</v>
       </c>
       <c r="P51" s="2"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -3036,31 +3090,31 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="7" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="P52" s="2"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -3068,31 +3122,31 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2" t="s">
-        <v>192</v>
+        <v>329</v>
       </c>
       <c r="P53" s="2"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -3100,24 +3154,24 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2" t="s">
-        <v>193</v>
+        <v>330</v>
       </c>
       <c r="P54" s="2"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>16</v>
       </c>
@@ -3135,20 +3189,20 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="P55" s="2"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>14</v>
@@ -3158,31 +3212,31 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2" t="s">
-        <v>199</v>
+        <v>331</v>
       </c>
       <c r="P56" s="2"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>14</v>
@@ -3192,31 +3246,31 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2" t="s">
-        <v>200</v>
+        <v>332</v>
       </c>
       <c r="P57" s="2"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -3224,31 +3278,31 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2" t="s">
-        <v>201</v>
+        <v>333</v>
       </c>
       <c r="P58" s="2"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -3256,31 +3310,31 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2" t="s">
-        <v>202</v>
+        <v>334</v>
       </c>
       <c r="P59" s="2"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -3288,24 +3342,24 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
       <c r="P60" s="2"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>16</v>
       </c>
@@ -3323,22 +3377,22 @@
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="P61" s="2"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>14</v>
@@ -3348,31 +3402,31 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2" t="s">
-        <v>226</v>
+        <v>336</v>
       </c>
       <c r="P62" s="2"/>
     </row>
-    <row r="63" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -3380,24 +3434,24 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2" t="s">
-        <v>231</v>
+        <v>337</v>
       </c>
       <c r="P63" s="2"/>
     </row>
-    <row r="64" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3408,27 +3462,27 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -3436,31 +3490,31 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" s="2" t="s">
-        <v>227</v>
+        <v>338</v>
       </c>
       <c r="P65" s="2"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -3468,31 +3522,31 @@
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2" t="s">
-        <v>232</v>
+        <v>339</v>
       </c>
       <c r="P66" s="2"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -3500,31 +3554,31 @@
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2" t="s">
-        <v>228</v>
+        <v>340</v>
       </c>
       <c r="P67" s="2"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -3532,31 +3586,31 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2" t="s">
-        <v>229</v>
+        <v>341</v>
       </c>
       <c r="P68" s="2"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -3564,24 +3618,24 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2" t="s">
-        <v>230</v>
+        <v>342</v>
       </c>
       <c r="P69" s="2"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>16</v>
       </c>
@@ -3599,22 +3653,22 @@
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="P70" s="2"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>14</v>
@@ -3629,18 +3683,18 @@
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" s="2" t="s">
-        <v>235</v>
+        <v>343</v>
       </c>
       <c r="P71" s="2"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>242</v>
+        <v>201</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>242</v>
+        <v>201</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>14</v>
@@ -3655,18 +3709,18 @@
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2" t="s">
-        <v>236</v>
+        <v>344</v>
       </c>
       <c r="P72" s="2"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>14</v>
@@ -3681,18 +3735,18 @@
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2" t="s">
-        <v>237</v>
+        <v>345</v>
       </c>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>14</v>
@@ -3707,18 +3761,18 @@
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2" t="s">
-        <v>255</v>
+        <v>346</v>
       </c>
       <c r="P74" s="2"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>239</v>
+        <v>198</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>239</v>
+        <v>198</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>14</v>
@@ -3733,18 +3787,18 @@
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2" t="s">
-        <v>239</v>
+        <v>347</v>
       </c>
       <c r="P75" s="2"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>240</v>
+        <v>199</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>240</v>
+        <v>199</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>14</v>
@@ -3759,18 +3813,18 @@
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2" t="s">
-        <v>240</v>
+        <v>348</v>
       </c>
       <c r="P76" s="2"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -3778,33 +3832,33 @@
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2" t="s">
-        <v>256</v>
+        <v>214</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>257</v>
+        <v>215</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>258</v>
+        <v>349</v>
       </c>
       <c r="P77" s="2"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>244</v>
+        <v>203</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>244</v>
+        <v>203</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -3812,22 +3866,22 @@
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2" t="s">
-        <v>259</v>
+        <v>216</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2" t="s">
-        <v>262</v>
+        <v>350</v>
       </c>
       <c r="P78" s="2"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3838,31 +3892,31 @@
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>257</v>
+        <v>215</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>245</v>
+        <v>204</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>245</v>
+        <v>204</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -3875,18 +3929,18 @@
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2" t="s">
-        <v>245</v>
+        <v>351</v>
       </c>
       <c r="P80" s="2"/>
     </row>
-    <row r="81" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>246</v>
+        <v>205</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>246</v>
+        <v>205</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -3899,18 +3953,18 @@
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2" t="s">
-        <v>246</v>
+        <v>352</v>
       </c>
       <c r="P81" s="2"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>247</v>
+        <v>206</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>247</v>
+        <v>206</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -3918,22 +3972,22 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2" t="s">
-        <v>264</v>
+        <v>220</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2" t="s">
-        <v>265</v>
+        <v>221</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>266</v>
+        <v>353</v>
       </c>
       <c r="P82" s="2"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>16</v>
       </c>
@@ -3951,689 +4005,694 @@
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" t="s">
-        <v>263</v>
+        <v>219</v>
       </c>
       <c r="P83" s="2"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>248</v>
+        <v>207</v>
       </c>
       <c r="C84" t="s">
-        <v>249</v>
+        <v>208</v>
       </c>
       <c r="D84" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="E84" t="s">
         <v>14</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="C85" t="s">
-        <v>250</v>
+        <v>209</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>272</v>
+        <v>227</v>
       </c>
       <c r="E85" t="s">
         <v>14</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C86" t="s">
-        <v>251</v>
+        <v>210</v>
       </c>
       <c r="D86" t="s">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C87" t="s">
-        <v>252</v>
+        <v>211</v>
       </c>
       <c r="D87" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C88" t="s">
-        <v>253</v>
+        <v>212</v>
       </c>
       <c r="D88" t="s">
-        <v>253</v>
+        <v>212</v>
       </c>
       <c r="O88" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>16</v>
       </c>
       <c r="O89" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="C90" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C91" t="s">
-        <v>274</v>
+        <v>229</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>278</v>
+        <v>233</v>
       </c>
       <c r="J91" t="s">
-        <v>279</v>
+        <v>234</v>
       </c>
       <c r="K91" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="L91" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="O91" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="C92" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="J92" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
       <c r="K92" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="N92" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
       <c r="O92" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D93" s="1"/>
       <c r="J93" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
       <c r="K93" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="N93" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
       <c r="O93" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C94" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>16</v>
       </c>
       <c r="O95" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>289</v>
+        <v>241</v>
       </c>
       <c r="B96" t="s">
         <v>14</v>
       </c>
       <c r="C96" t="s">
-        <v>290</v>
+        <v>242</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>290</v>
+        <v>242</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C97" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="D97" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:15" ht="29" x14ac:dyDescent="0.35">
       <c r="C98" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
       <c r="D98" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
       <c r="J98" t="s">
-        <v>304</v>
+        <v>256</v>
       </c>
       <c r="K98" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L98" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M98" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="O98" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="99" spans="3:15" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="99" spans="3:15" x14ac:dyDescent="0.35">
       <c r="J99" t="s">
-        <v>308</v>
+        <v>259</v>
       </c>
       <c r="K99" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="100" spans="3:15" ht="45" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="100" spans="3:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="J100" t="s">
-        <v>309</v>
+        <v>260</v>
       </c>
       <c r="K100" t="s">
-        <v>305</v>
+        <v>257</v>
       </c>
       <c r="L100" t="s">
-        <v>305</v>
+        <v>257</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="101" spans="3:15" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="101" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
-        <v>310</v>
+        <v>261</v>
       </c>
       <c r="D101" t="s">
-        <v>310</v>
+        <v>261</v>
       </c>
       <c r="J101" t="s">
-        <v>311</v>
+        <v>262</v>
       </c>
       <c r="K101" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="N101" t="s">
-        <v>323</v>
+        <v>272</v>
       </c>
       <c r="O101" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="102" spans="3:15" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="102" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C102" t="s">
-        <v>293</v>
+        <v>245</v>
       </c>
       <c r="D102" t="s">
-        <v>293</v>
+        <v>245</v>
       </c>
       <c r="J102" t="s">
-        <v>312</v>
+        <v>263</v>
       </c>
       <c r="K102" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="O102" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="103" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="103" spans="3:15" ht="29" x14ac:dyDescent="0.35">
       <c r="C103" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="D103" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="J103" t="s">
-        <v>313</v>
+        <v>264</v>
       </c>
       <c r="K103" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="O103" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="104" spans="3:15" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="104" spans="3:15" x14ac:dyDescent="0.35">
       <c r="J104" t="s">
-        <v>314</v>
+        <v>265</v>
       </c>
       <c r="K104" t="s">
-        <v>324</v>
+        <v>273</v>
       </c>
       <c r="L104" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="105" spans="3:15" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="105" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
-        <v>295</v>
+        <v>247</v>
       </c>
       <c r="D105" t="s">
-        <v>295</v>
+        <v>247</v>
       </c>
       <c r="J105" t="s">
-        <v>315</v>
+        <v>266</v>
       </c>
       <c r="K105" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="O105" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="106" spans="3:15" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="106" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
-        <v>296</v>
+        <v>248</v>
       </c>
       <c r="D106" t="s">
-        <v>296</v>
+        <v>248</v>
       </c>
       <c r="J106" t="s">
-        <v>316</v>
+        <v>267</v>
       </c>
       <c r="K106" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="O106" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="107" spans="3:15" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="107" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="D107" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="J107" t="s">
-        <v>317</v>
+        <v>268</v>
       </c>
       <c r="K107" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="L107" s="2" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="O107" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="108" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="108" spans="3:15" ht="29" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
-        <v>298</v>
+        <v>250</v>
       </c>
       <c r="D108" t="s">
-        <v>298</v>
+        <v>250</v>
       </c>
       <c r="J108" t="s">
-        <v>318</v>
+        <v>269</v>
       </c>
       <c r="K108" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="109" spans="3:15" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="109" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="D109" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="O109" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="110" spans="3:15" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="110" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
       <c r="D110" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
       <c r="O110" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="111" spans="3:15" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="111" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
       <c r="D111" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
       <c r="O111" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="112" spans="3:15" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="112" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C112" t="s">
-        <v>302</v>
+        <v>254</v>
       </c>
       <c r="D112" t="s">
-        <v>302</v>
+        <v>254</v>
       </c>
       <c r="O112" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>16</v>
       </c>
       <c r="O113" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>303</v>
+        <v>255</v>
       </c>
       <c r="C114" t="s">
-        <v>361</v>
+        <v>298</v>
       </c>
       <c r="D114" t="s">
-        <v>332</v>
+        <v>275</v>
       </c>
       <c r="E114" t="s">
         <v>14</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C115" t="s">
-        <v>333</v>
+        <v>276</v>
       </c>
       <c r="D115" t="s">
-        <v>333</v>
+        <v>276</v>
       </c>
       <c r="J115" t="s">
-        <v>335</v>
+        <v>278</v>
       </c>
       <c r="K115" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L115" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M115" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="O115" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C116" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
       <c r="D116" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
       <c r="J116" t="s">
-        <v>336</v>
+        <v>279</v>
       </c>
       <c r="K116" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L116" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M116" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="O116" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
-        <v>346</v>
+        <v>286</v>
       </c>
       <c r="D117" t="s">
-        <v>346</v>
+        <v>286</v>
       </c>
       <c r="J117" t="s">
-        <v>337</v>
+        <v>280</v>
       </c>
       <c r="K117" t="s">
-        <v>338</v>
+        <v>281</v>
       </c>
       <c r="N117" t="s">
-        <v>339</v>
+        <v>282</v>
       </c>
       <c r="O117" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>16</v>
       </c>
       <c r="O118" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>344</v>
+        <v>284</v>
       </c>
       <c r="C119" t="s">
-        <v>361</v>
+        <v>298</v>
       </c>
       <c r="D119" t="s">
-        <v>345</v>
+        <v>285</v>
       </c>
       <c r="O119" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C120" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
       <c r="D120" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
       <c r="J120" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
       <c r="K120" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L120" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M120" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="O120" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C121" t="s">
-        <v>348</v>
+        <v>288</v>
       </c>
       <c r="D121" t="s">
-        <v>348</v>
+        <v>288</v>
       </c>
       <c r="J121" t="s">
-        <v>353</v>
+        <v>291</v>
       </c>
       <c r="N121" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="O121" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>16</v>
       </c>
       <c r="O122" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>355</v>
+        <v>292</v>
       </c>
       <c r="C123" t="s">
-        <v>361</v>
+        <v>298</v>
       </c>
       <c r="D123" t="s">
-        <v>357</v>
+        <v>294</v>
       </c>
       <c r="E123" t="s">
         <v>14</v>
       </c>
       <c r="O123" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C124" t="s">
-        <v>358</v>
+        <v>295</v>
       </c>
       <c r="D124" t="s">
-        <v>358</v>
+        <v>295</v>
       </c>
       <c r="J124" t="s">
-        <v>366</v>
+        <v>302</v>
       </c>
       <c r="K124" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L124" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="O124" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="125" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="C125" t="s">
-        <v>359</v>
+        <v>296</v>
       </c>
       <c r="D125" t="s">
-        <v>359</v>
+        <v>296</v>
       </c>
       <c r="J125" t="s">
-        <v>365</v>
+        <v>301</v>
       </c>
       <c r="K125" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="L125" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="M125" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>363</v>
+        <v>300</v>
       </c>
       <c r="O125" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C126" t="s">
-        <v>360</v>
+        <v>297</v>
       </c>
       <c r="D126" t="s">
-        <v>360</v>
+        <v>297</v>
       </c>
       <c r="J126" t="s">
-        <v>367</v>
+        <v>303</v>
       </c>
       <c r="K126" t="s">
-        <v>362</v>
+        <v>299</v>
       </c>
       <c r="L126" t="s">
-        <v>362</v>
+        <v>299</v>
       </c>
       <c r="O126" t="s">
-        <v>368</v>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -4644,15 +4703,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B662EE53BAED864D9E45A03F917DD171" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0b478698d34ba6ea8d28dcb235cef59d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac726c7a-29b1-4eed-9efa-e398fb837db4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0bae4f718acc166ce461856f4d6d984a" ns3:_="">
     <xsd:import namespace="ac726c7a-29b1-4eed-9efa-e398fb837db4"/>
@@ -4798,6 +4848,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4805,14 +4864,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368DB8FB-3FF0-4C81-B088-BE74BE0C63EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1CA99AA-BB55-4566-A33D-E268FF599705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4826,6 +4877,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368DB8FB-3FF0-4C81-B088-BE74BE0C63EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>